<commit_message>
edited Rover lego design
</commit_message>
<xml_diff>
--- a/Lego/car-BOM.xlsx
+++ b/Lego/car-BOM.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>Brick</t>
   </si>
@@ -135,12 +135,6 @@
   </si>
   <si>
     <t>CONNECTOR PEG</t>
-  </si>
-  <si>
-    <t>451926</t>
-  </si>
-  <si>
-    <t>CROSS AXLE 3M</t>
   </si>
   <si>
     <t>4225927</t>
@@ -1021,7 +1015,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="451926 Screenshot" descr="451926"/>
+        <xdr:cNvPr id="19" name="4225927 Screenshot" descr="4225927"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1065,7 +1059,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="4225927 Screenshot" descr="4225927"/>
+        <xdr:cNvPr id="20" name="4141814 Screenshot" descr="4141814"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1109,7 +1103,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="4141814 Screenshot" descr="4141814"/>
+        <xdr:cNvPr id="21" name="4189110 Screenshot" descr="4189110"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1153,7 +1147,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="4189110 Screenshot" descr="4189110"/>
+        <xdr:cNvPr id="22" name="4514553 Screenshot" descr="4514553"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1197,7 +1191,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="4514553 Screenshot" descr="4514553"/>
+        <xdr:cNvPr id="23" name="4164357 Screenshot" descr="4164357"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1241,7 +1235,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="4164357 Screenshot" descr="4164357"/>
+        <xdr:cNvPr id="24" name="4227273 Screenshot" descr="4227273"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1285,7 +1279,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="4227273 Screenshot" descr="4227273"/>
+        <xdr:cNvPr id="25" name="370626 Screenshot" descr="370626"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1329,7 +1323,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="370626 Screenshot" descr="370626"/>
+        <xdr:cNvPr id="26" name="4185111 Screenshot" descr="4185111"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1373,7 +1367,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="4185111 Screenshot" descr="4185111"/>
+        <xdr:cNvPr id="27" name="4124045 Screenshot" descr="4124045"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1417,7 +1411,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="4124045 Screenshot" descr="4124045"/>
+        <xdr:cNvPr id="28" name="4114670 Screenshot" descr="4114670"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1461,7 +1455,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="4114670 Screenshot" descr="4114670"/>
+        <xdr:cNvPr id="29" name="4195018 Screenshot" descr="4195018"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1505,7 +1499,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="4195018 Screenshot" descr="4195018"/>
+        <xdr:cNvPr id="30" name="4158925 Screenshot" descr="4158925"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1549,7 +1543,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="4158925 Screenshot" descr="4158925"/>
+        <xdr:cNvPr id="31" name="6043747 Screenshot" descr="6043747"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1593,7 +1587,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="6043747 Screenshot" descr="6043747"/>
+        <xdr:cNvPr id="32" name="4114671 Screenshot" descr="4114671"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1637,7 +1631,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="4114671 Screenshot" descr="4114671"/>
+        <xdr:cNvPr id="33" name="4141806 Screenshot" descr="4141806"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1681,7 +1675,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="4141806 Screenshot" descr="4141806"/>
+        <xdr:cNvPr id="34" name="3226901 Screenshot" descr="3226901"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1725,7 +1719,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="3226901 Screenshot" descr="3226901"/>
+        <xdr:cNvPr id="35" name="4525184 Screenshot" descr="4525184"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1745,50 +1739,6 @@
       <xdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="3448050" y="28698825"/>
-          <a:ext cx="813600" cy="813600"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>812800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="4525184 Screenshot" descr="4525184"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image35">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3448050" y="29537025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -1803,7 +1753,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1985,7 +1935,7 @@
         <v>17</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="66" customHeight="1">
@@ -2002,7 +1952,7 @@
         <v>11</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="66" customHeight="1">
@@ -2019,7 +1969,7 @@
         <v>14</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="66" customHeight="1">
@@ -2036,7 +1986,7 @@
         <v>17</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="66" customHeight="1">
@@ -2104,7 +2054,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="66" customHeight="1">
@@ -2121,7 +2071,7 @@
         <v>14</v>
       </c>
       <c r="F18">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="66" customHeight="1">
@@ -2132,13 +2082,13 @@
         <v>43</v>
       </c>
       <c r="D19">
-        <v>4519</v>
+        <v>6562</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="66" customHeight="1">
@@ -2149,13 +2099,13 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>6562</v>
+        <v>6590</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" customHeight="1">
@@ -2166,13 +2116,13 @@
         <v>47</v>
       </c>
       <c r="D21">
-        <v>6590</v>
+        <v>43093</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="66" customHeight="1">
@@ -2183,13 +2133,13 @@
         <v>49</v>
       </c>
       <c r="D22">
-        <v>43093</v>
+        <v>6558</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="66" customHeight="1">
@@ -2200,13 +2150,13 @@
         <v>51</v>
       </c>
       <c r="D23">
-        <v>6558</v>
+        <v>32039</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="66" customHeight="1">
@@ -2217,7 +2167,7 @@
         <v>53</v>
       </c>
       <c r="D24">
-        <v>32039</v>
+        <v>6536</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
@@ -2234,13 +2184,13 @@
         <v>55</v>
       </c>
       <c r="D25">
-        <v>6536</v>
+        <v>3706</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="66" customHeight="1">
@@ -2251,13 +2201,13 @@
         <v>57</v>
       </c>
       <c r="D26">
-        <v>3706</v>
+        <v>44294</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="66" customHeight="1">
@@ -2268,13 +2218,13 @@
         <v>59</v>
       </c>
       <c r="D27">
-        <v>44294</v>
+        <v>59426</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="66" customHeight="1">
@@ -2285,7 +2235,7 @@
         <v>61</v>
       </c>
       <c r="D28">
-        <v>59426</v>
+        <v>32068</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -2302,13 +2252,13 @@
         <v>63</v>
       </c>
       <c r="D29">
-        <v>32068</v>
+        <v>44809</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="66" customHeight="1">
@@ -2319,13 +2269,13 @@
         <v>65</v>
       </c>
       <c r="D30">
-        <v>44809</v>
+        <v>32557</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F30">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="66" customHeight="1">
@@ -2336,13 +2286,13 @@
         <v>67</v>
       </c>
       <c r="D31">
-        <v>32557</v>
+        <v>50451</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F31">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="66" customHeight="1">
@@ -2353,13 +2303,13 @@
         <v>69</v>
       </c>
       <c r="D32">
-        <v>50451</v>
+        <v>32069</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="66" customHeight="1">
@@ -2370,30 +2320,30 @@
         <v>71</v>
       </c>
       <c r="D33">
-        <v>32069</v>
+        <v>6589</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="66" customHeight="1">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D34">
-        <v>6589</v>
+        <v>32269</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="66" customHeight="1">
@@ -2404,38 +2354,21 @@
         <v>76</v>
       </c>
       <c r="D35">
-        <v>32269</v>
+        <v>62821</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="66" customHeight="1">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" t="s">
         <v>78</v>
       </c>
-      <c r="D36">
-        <v>62821</v>
-      </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
       <c r="F36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37">
-        <f>SUM(F2:F36)</f>
+        <f>SUM(F2:F35)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited Lego design - removed differential
</commit_message>
<xml_diff>
--- a/Lego/car-BOM.xlsx
+++ b/Lego/car-BOM.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Brick</t>
   </si>
@@ -137,6 +137,12 @@
     <t>CONNECTOR PEG</t>
   </si>
   <si>
+    <t>451926</t>
+  </si>
+  <si>
+    <t>CROSS AXLE 3M</t>
+  </si>
+  <si>
     <t>4225927</t>
   </si>
   <si>
@@ -161,6 +167,15 @@
     <t>CONNECTOR PEG W. FRICTION 3M</t>
   </si>
   <si>
+    <t>4512360</t>
+  </si>
+  <si>
+    <t>CROSS AXLE, EXTENSION, 2M</t>
+  </si>
+  <si>
+    <t>194 - Medium Stone Grey</t>
+  </si>
+  <si>
     <t>4164357</t>
   </si>
   <si>
@@ -185,6 +200,12 @@
     <t>CROSS AXLE 7M</t>
   </si>
   <si>
+    <t>370726</t>
+  </si>
+  <si>
+    <t>CROSS AXLE 8M</t>
+  </si>
+  <si>
     <t>4124045</t>
   </si>
   <si>
@@ -209,40 +230,22 @@
     <t>TECHNIC CROSSBLOCK 2X3</t>
   </si>
   <si>
-    <t>6043747</t>
-  </si>
-  <si>
-    <t>16M AXLE Ø 4.75 W. CROSS</t>
-  </si>
-  <si>
     <t>4114671</t>
   </si>
   <si>
     <t>T. STEERING GEAR, BEARING 2M</t>
   </si>
   <si>
-    <t>4141806</t>
-  </si>
-  <si>
-    <t>CONICAL WHEEL Z12</t>
-  </si>
-  <si>
-    <t>24 - Bright Yellow</t>
-  </si>
-  <si>
     <t>3226901</t>
   </si>
   <si>
     <t>DOUBLE CONICAL WHEEL Z20 1M</t>
   </si>
   <si>
-    <t>4525184</t>
-  </si>
-  <si>
-    <t>DIFFERENTIALE 3M Z 28</t>
-  </si>
-  <si>
-    <t>199 - Dark Stone Grey</t>
+    <t>4211434</t>
+  </si>
+  <si>
+    <t>CROWN- AND GEAR WHEEL Z24</t>
   </si>
   <si>
     <t>Total:</t>
@@ -1015,7 +1018,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="4225927 Screenshot" descr="4225927"/>
+        <xdr:cNvPr id="19" name="451926 Screenshot" descr="451926"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1059,7 +1062,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="4141814 Screenshot" descr="4141814"/>
+        <xdr:cNvPr id="20" name="4225927 Screenshot" descr="4225927"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1103,7 +1106,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="4189110 Screenshot" descr="4189110"/>
+        <xdr:cNvPr id="21" name="4141814 Screenshot" descr="4141814"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1147,7 +1150,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="4514553 Screenshot" descr="4514553"/>
+        <xdr:cNvPr id="22" name="4189110 Screenshot" descr="4189110"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1191,7 +1194,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="4164357 Screenshot" descr="4164357"/>
+        <xdr:cNvPr id="23" name="4514553 Screenshot" descr="4514553"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1235,7 +1238,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="4227273 Screenshot" descr="4227273"/>
+        <xdr:cNvPr id="24" name="4512360 Screenshot" descr="4512360"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1279,7 +1282,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="370626 Screenshot" descr="370626"/>
+        <xdr:cNvPr id="25" name="4164357 Screenshot" descr="4164357"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1323,7 +1326,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="4185111 Screenshot" descr="4185111"/>
+        <xdr:cNvPr id="26" name="4227273 Screenshot" descr="4227273"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1367,7 +1370,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="4124045 Screenshot" descr="4124045"/>
+        <xdr:cNvPr id="27" name="370626 Screenshot" descr="370626"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1411,7 +1414,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="4114670 Screenshot" descr="4114670"/>
+        <xdr:cNvPr id="28" name="4185111 Screenshot" descr="4185111"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1455,7 +1458,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="4195018 Screenshot" descr="4195018"/>
+        <xdr:cNvPr id="29" name="370726 Screenshot" descr="370726"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1499,7 +1502,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="4158925 Screenshot" descr="4158925"/>
+        <xdr:cNvPr id="30" name="4124045 Screenshot" descr="4124045"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1543,7 +1546,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="6043747 Screenshot" descr="6043747"/>
+        <xdr:cNvPr id="31" name="4114670 Screenshot" descr="4114670"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1587,7 +1590,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="4114671 Screenshot" descr="4114671"/>
+        <xdr:cNvPr id="32" name="4195018 Screenshot" descr="4195018"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1631,7 +1634,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="4141806 Screenshot" descr="4141806"/>
+        <xdr:cNvPr id="33" name="4158925 Screenshot" descr="4158925"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1675,7 +1678,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="3226901 Screenshot" descr="3226901"/>
+        <xdr:cNvPr id="34" name="4114671 Screenshot" descr="4114671"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1719,7 +1722,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="4525184 Screenshot" descr="4525184"/>
+        <xdr:cNvPr id="35" name="3226901 Screenshot" descr="3226901"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1739,6 +1742,50 @@
       <xdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="3448050" y="28698825"/>
+          <a:ext cx="813600" cy="813600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>812800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="4211434 Screenshot" descr="4211434"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image35">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3448050" y="29537025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -1753,7 +1800,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2054,7 +2101,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="66" customHeight="1">
@@ -2082,13 +2129,13 @@
         <v>43</v>
       </c>
       <c r="D19">
-        <v>6562</v>
+        <v>4519</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="66" customHeight="1">
@@ -2099,13 +2146,13 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>6590</v>
+        <v>6562</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="66" customHeight="1">
@@ -2116,13 +2163,13 @@
         <v>47</v>
       </c>
       <c r="D21">
-        <v>43093</v>
+        <v>6590</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="66" customHeight="1">
@@ -2133,13 +2180,13 @@
         <v>49</v>
       </c>
       <c r="D22">
-        <v>6558</v>
+        <v>43093</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="66" customHeight="1">
@@ -2150,13 +2197,13 @@
         <v>51</v>
       </c>
       <c r="D23">
-        <v>32039</v>
+        <v>6558</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="66" customHeight="1">
@@ -2167,44 +2214,44 @@
         <v>53</v>
       </c>
       <c r="D24">
-        <v>6536</v>
+        <v>59443</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="66" customHeight="1">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25">
-        <v>3706</v>
+        <v>32039</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="66" customHeight="1">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D26">
-        <v>44294</v>
+        <v>6536</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2212,13 +2259,13 @@
     </row>
     <row r="27" spans="1:6" ht="66" customHeight="1">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D27">
-        <v>59426</v>
+        <v>3706</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -2229,104 +2276,104 @@
     </row>
     <row r="28" spans="1:6" ht="66" customHeight="1">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D28">
-        <v>32068</v>
+        <v>44294</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="66" customHeight="1">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D29">
-        <v>44809</v>
+        <v>3707</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F29">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="66" customHeight="1">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30">
-        <v>32557</v>
+        <v>59426</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="66" customHeight="1">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31">
-        <v>50451</v>
+        <v>32068</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="66" customHeight="1">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32">
-        <v>32069</v>
+        <v>44809</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="66" customHeight="1">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D33">
-        <v>6589</v>
+        <v>32557</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="F33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="66" customHeight="1">
@@ -2337,13 +2384,13 @@
         <v>74</v>
       </c>
       <c r="D34">
-        <v>32269</v>
+        <v>32069</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="66" customHeight="1">
@@ -2354,21 +2401,38 @@
         <v>76</v>
       </c>
       <c r="D35">
-        <v>62821</v>
+        <v>32269</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" ht="66" customHeight="1">
       <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
         <v>78</v>
       </c>
+      <c r="D36">
+        <v>3650</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
       <c r="F36">
-        <f>SUM(F2:F35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37">
+        <f>SUM(F2:F36)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>